<commit_message>
Fixed issue with missing primer reporting
</commit_message>
<xml_diff>
--- a/ddprimer/test_data/Primers/Primers_Sequences.xlsx
+++ b/ddprimer/test_data/Primers/Primers_Sequences.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -654,19 +654,19 @@
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>T-complex protein 11</t>
+          <t>ALDH3H1</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>CTTCTTAAGGGACCTGCTG</t>
+          <t>TGTCCCACTTCTGCTCTAG</t>
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>57.12484309067128</v>
+        <v>58.01484146521688</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>1.440946383012932</v>
+        <v>1.580630938901084</v>
       </c>
       <c r="E3" s="6" t="n">
         <v>0</v>
@@ -679,14 +679,14 @@
       </c>
       <c r="H3" s="7" t="inlineStr">
         <is>
-          <t>CAATGGTAGCGAGGAAGAC</t>
+          <t>GTCAGCTCTGCTCACTAAG</t>
         </is>
       </c>
       <c r="I3" s="6" t="n">
-        <v>57.62652924333611</v>
+        <v>57.25780068211964</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>1.192318717020317</v>
+        <v>1.307988791564572</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>0</v>
@@ -698,280 +698,622 @@
         <v>1.1</v>
       </c>
       <c r="N3" s="6" t="n">
-        <v>2.633265100033249</v>
+        <v>2.888619730465656</v>
       </c>
       <c r="O3" s="7" t="inlineStr">
         <is>
-          <t>CCAGTCGGCATGGTTCCCCAGACCA</t>
+          <t>AGCTCCTTCGACAACTCGCACCGCA</t>
         </is>
       </c>
       <c r="P3" s="6" t="n">
-        <v>64.11130686824305</v>
+        <v>64.49642205565243</v>
       </c>
       <c r="Q3" s="6" t="n">
-        <v>5.888693131756952</v>
+        <v>5.503577944347569</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>-0.3405189514160156</v>
+        <v>0</v>
       </c>
       <c r="S3" s="6" t="n">
         <v>3.95e-06</v>
       </c>
       <c r="T3" s="6" t="n">
-        <v>0.08699999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="U3" s="7" t="inlineStr">
         <is>
-          <t>CTTCTTAAGGGACCTGCTGGTCTGGAATATCTGAAGAAGTCATTTTCCAGTCGGCATGGTTCCCCAGACCAAGCGTCTTCCTCGCTACCATTG</t>
+          <t>TGTCCCACTTCTGCTCTAGCAGAGCACTTGTTTCGGTAACAGCTCCTTCGACAACTCGCACCGCAGAAGGATCAAGATACTGTTCCAGTAACTTAGTGAGCAGAGCTGAC</t>
         </is>
       </c>
       <c r="V3" s="6" t="n">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="W3" s="6" t="n">
-        <v>50.53763440860215</v>
+        <v>50</v>
       </c>
       <c r="X3" s="6" t="n">
-        <v>-6.266936302185059</v>
+        <v>-6.408234596252441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
-          <t>ALDH3H1</t>
-        </is>
-      </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr"/>
-      <c r="D4" s="6" t="inlineStr"/>
-      <c r="E4" s="6" t="inlineStr"/>
-      <c r="F4" s="6" t="inlineStr"/>
-      <c r="G4" s="6" t="inlineStr"/>
-      <c r="H4" s="7" t="inlineStr"/>
-      <c r="I4" s="6" t="inlineStr"/>
-      <c r="J4" s="6" t="inlineStr"/>
-      <c r="K4" s="6" t="inlineStr"/>
-      <c r="L4" s="6" t="inlineStr"/>
-      <c r="M4" s="6" t="inlineStr"/>
-      <c r="N4" s="6" t="inlineStr"/>
-      <c r="O4" s="7" t="inlineStr"/>
-      <c r="P4" s="6" t="inlineStr"/>
-      <c r="Q4" s="6" t="inlineStr"/>
-      <c r="R4" s="6" t="inlineStr"/>
-      <c r="S4" s="6" t="inlineStr"/>
-      <c r="T4" s="6" t="inlineStr"/>
-      <c r="U4" s="7" t="inlineStr"/>
-      <c r="V4" s="6" t="inlineStr"/>
-      <c r="W4" s="6" t="inlineStr"/>
-      <c r="X4" s="6" t="inlineStr"/>
+          <t>SEU</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>GGATACAAGTGGTGCTGAG</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>57.52962325587004</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1.095412729554244</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>CCCTGAACTTGACCTGATG</t>
+        </is>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>57.43104509705881</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>1.134744376625395</v>
+      </c>
+      <c r="K4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N4" s="6" t="n">
+        <v>2.230157106179639</v>
+      </c>
+      <c r="O4" s="7" t="inlineStr">
+        <is>
+          <t>GCGCGGAGACACCATACTCGACGCA</t>
+        </is>
+      </c>
+      <c r="P4" s="6" t="n">
+        <v>64.84823406353087</v>
+      </c>
+      <c r="Q4" s="6" t="n">
+        <v>5.151765936469133</v>
+      </c>
+      <c r="R4" s="6" t="n">
+        <v>-1.205482959747314</v>
+      </c>
+      <c r="S4" s="6" t="n">
+        <v>3.95e-06</v>
+      </c>
+      <c r="T4" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U4" s="7" t="inlineStr">
+        <is>
+          <t>GGATACAAGTGGTGCTGAGTCTGACCCGATGTCTAACGTCGGGTTTAGTGGTTTGTCGTCTTTTAATGCGTCGAGTATGGTGTCTCCGCGCTCATCAGGTCAAGTTCAGGG</t>
+        </is>
+      </c>
+      <c r="V4" s="6" t="n">
+        <v>111</v>
+      </c>
+      <c r="W4" s="6" t="n">
+        <v>51.35135135135135</v>
+      </c>
+      <c r="X4" s="6" t="n">
+        <v>-4.978288650512695</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
-          <t>SEU</t>
-        </is>
-      </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr"/>
-      <c r="D5" s="6" t="inlineStr"/>
-      <c r="E5" s="6" t="inlineStr"/>
-      <c r="F5" s="6" t="inlineStr"/>
+          <t>ILL6</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>CAAGAGGACTAGCTTCACG</t>
+        </is>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>57.26560667118389</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>1.30018280250032</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>0.007</v>
+      </c>
       <c r="G5" s="6" t="inlineStr"/>
-      <c r="H5" s="7" t="inlineStr"/>
-      <c r="I5" s="6" t="inlineStr"/>
-      <c r="J5" s="6" t="inlineStr"/>
-      <c r="K5" s="6" t="inlineStr"/>
-      <c r="L5" s="6" t="inlineStr"/>
-      <c r="M5" s="6" t="inlineStr"/>
-      <c r="N5" s="6" t="inlineStr"/>
-      <c r="O5" s="7" t="inlineStr"/>
-      <c r="P5" s="6" t="inlineStr"/>
-      <c r="Q5" s="6" t="inlineStr"/>
-      <c r="R5" s="6" t="inlineStr"/>
-      <c r="S5" s="6" t="inlineStr"/>
-      <c r="T5" s="6" t="inlineStr"/>
-      <c r="U5" s="7" t="inlineStr"/>
-      <c r="V5" s="6" t="inlineStr"/>
-      <c r="W5" s="6" t="inlineStr"/>
-      <c r="X5" s="6" t="inlineStr"/>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>GTCCCATATCCATCCAACG</t>
+        </is>
+      </c>
+      <c r="I5" s="6" t="n">
+        <v>57.36368514341291</v>
+      </c>
+      <c r="J5" s="6" t="n">
+        <v>1.2021043302713</v>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N5" s="6" t="n">
+        <v>2.50228713277162</v>
+      </c>
+      <c r="O5" s="7" t="inlineStr">
+        <is>
+          <t>AGCGGCGCCACGGCTATCTTCCG</t>
+        </is>
+      </c>
+      <c r="P5" s="6" t="n">
+        <v>65.57831797103955</v>
+      </c>
+      <c r="Q5" s="6" t="n">
+        <v>3.578317971039553</v>
+      </c>
+      <c r="R5" s="6" t="n">
+        <v>-1.226303815841675</v>
+      </c>
+      <c r="S5" s="6" t="n">
+        <v>4.81e-05</v>
+      </c>
+      <c r="T5" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U5" s="7" t="inlineStr">
+        <is>
+          <t>CAAGAGGACTAGCTTCACGGGATACAATGCCTTGAAGACTAATGACCGCGGAAGAAGCTGCAAGAAGGAGATTAGCGGCGCCACGGCTATCTTCCGAAGTGATAACCGCCCGGAAAATTCCACATCCCGCGAGCAAAGGACCACTTCTTGATCCAATCACACCCGTTGGATGGATATGGGAC</t>
+        </is>
+      </c>
+      <c r="V5" s="6" t="n">
+        <v>182</v>
+      </c>
+      <c r="W5" s="6" t="n">
+        <v>52.1978021978022</v>
+      </c>
+      <c r="X5" s="6" t="n">
+        <v>-12.88146591186523</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>ABF2</t>
-        </is>
-      </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C6" s="6" t="inlineStr"/>
-      <c r="D6" s="6" t="inlineStr"/>
-      <c r="E6" s="6" t="inlineStr"/>
-      <c r="F6" s="6" t="inlineStr"/>
-      <c r="G6" s="6" t="inlineStr"/>
-      <c r="H6" s="7" t="inlineStr"/>
-      <c r="I6" s="6" t="inlineStr"/>
-      <c r="J6" s="6" t="inlineStr"/>
-      <c r="K6" s="6" t="inlineStr"/>
-      <c r="L6" s="6" t="inlineStr"/>
-      <c r="M6" s="6" t="inlineStr"/>
-      <c r="N6" s="6" t="inlineStr"/>
-      <c r="O6" s="7" t="inlineStr"/>
-      <c r="P6" s="6" t="inlineStr"/>
-      <c r="Q6" s="6" t="inlineStr"/>
-      <c r="R6" s="6" t="inlineStr"/>
-      <c r="S6" s="6" t="inlineStr"/>
-      <c r="T6" s="6" t="inlineStr"/>
-      <c r="U6" s="7" t="inlineStr"/>
-      <c r="V6" s="6" t="inlineStr"/>
-      <c r="W6" s="6" t="inlineStr"/>
-      <c r="X6" s="6" t="inlineStr"/>
+          <t>ILL6</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>CTAATGACCGCGGAAGAAG</t>
+        </is>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>58.01929187670885</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1.585081350393057</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H6" s="7" t="inlineStr">
+        <is>
+          <t>CGGGTGTGATTGGATCAAG</t>
+        </is>
+      </c>
+      <c r="I6" s="6" t="n">
+        <v>58.21292292371351</v>
+      </c>
+      <c r="J6" s="6" t="n">
+        <v>1.778712397397715</v>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M6" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N6" s="6" t="n">
+        <v>3.363793747790773</v>
+      </c>
+      <c r="O6" s="7" t="inlineStr">
+        <is>
+          <t>AGCGGCGCCACGGCTATCTTCCG</t>
+        </is>
+      </c>
+      <c r="P6" s="6" t="n">
+        <v>65.57831797103955</v>
+      </c>
+      <c r="Q6" s="6" t="n">
+        <v>3.578317971039553</v>
+      </c>
+      <c r="R6" s="6" t="n">
+        <v>-1.226303815841675</v>
+      </c>
+      <c r="S6" s="6" t="n">
+        <v>4.81e-05</v>
+      </c>
+      <c r="T6" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U6" s="7" t="inlineStr">
+        <is>
+          <t>CTAATGACCGCGGAAGAAGCTGCAAGAAGGAGATTAGCGGCGCCACGGCTATCTTCCGAAGTGATAACCGCCCGGAAAATTCCACATCCCGCGAGCAAAGGACCACTTCTTGATCCAATCACACCCGT</t>
+        </is>
+      </c>
+      <c r="V6" s="6" t="n">
+        <v>127</v>
+      </c>
+      <c r="W6" s="6" t="n">
+        <v>53.90625</v>
+      </c>
+      <c r="X6" s="6" t="n">
+        <v>-7.592188835144043</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>MAPKKK9</t>
-        </is>
-      </c>
-      <c r="B7" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C7" s="6" t="inlineStr"/>
-      <c r="D7" s="6" t="inlineStr"/>
-      <c r="E7" s="6" t="inlineStr"/>
-      <c r="F7" s="6" t="inlineStr"/>
+          <t>ILL6</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>CTTCACGGGATACAATGCC</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>58.29104915522316</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>1.856838628907372</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>-0.4917802810668945</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>0.007</v>
+      </c>
       <c r="G7" s="6" t="inlineStr"/>
-      <c r="H7" s="7" t="inlineStr"/>
-      <c r="I7" s="6" t="inlineStr"/>
-      <c r="J7" s="6" t="inlineStr"/>
-      <c r="K7" s="6" t="inlineStr"/>
-      <c r="L7" s="6" t="inlineStr"/>
-      <c r="M7" s="6" t="inlineStr"/>
-      <c r="N7" s="6" t="inlineStr"/>
-      <c r="O7" s="7" t="inlineStr"/>
-      <c r="P7" s="6" t="inlineStr"/>
-      <c r="Q7" s="6" t="inlineStr"/>
-      <c r="R7" s="6" t="inlineStr"/>
-      <c r="S7" s="6" t="inlineStr"/>
-      <c r="T7" s="6" t="inlineStr"/>
-      <c r="U7" s="7" t="inlineStr"/>
-      <c r="V7" s="6" t="inlineStr"/>
-      <c r="W7" s="6" t="inlineStr"/>
-      <c r="X7" s="6" t="inlineStr"/>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>GCGGTTATCACTTCGGAAG</t>
+        </is>
+      </c>
+      <c r="I7" s="6" t="n">
+        <v>58.31982523388075</v>
+      </c>
+      <c r="J7" s="6" t="n">
+        <v>1.885614707564958</v>
+      </c>
+      <c r="K7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M7" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N7" s="6" t="n">
+        <v>3.74245333647233</v>
+      </c>
+      <c r="O7" s="7" t="inlineStr">
+        <is>
+          <t>CGTGGCGCCGCTAATCTCCTTCTTGCA</t>
+        </is>
+      </c>
+      <c r="P7" s="6" t="n">
+        <v>64.97929087626449</v>
+      </c>
+      <c r="Q7" s="6" t="n">
+        <v>7.020709123735514</v>
+      </c>
+      <c r="R7" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="6" t="n">
+        <v>5.4e-07</v>
+      </c>
+      <c r="T7" s="6" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="U7" s="7" t="inlineStr">
+        <is>
+          <t>CTTCACGGGATACAATGCCTTGAAGACTAATGACCGCGGAAGAAGCTGCAAGAAGGAGATTAGCGGCGCCACGGCTATCTTCCGAAGTGATAACCGCC</t>
+        </is>
+      </c>
+      <c r="V7" s="6" t="n">
+        <v>97</v>
+      </c>
+      <c r="W7" s="6" t="n">
+        <v>53.06122448979592</v>
+      </c>
+      <c r="X7" s="6" t="n">
+        <v>-8.713742256164551</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>GA20OX5</t>
-        </is>
-      </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C8" s="6" t="inlineStr"/>
-      <c r="D8" s="6" t="inlineStr"/>
-      <c r="E8" s="6" t="inlineStr"/>
-      <c r="F8" s="6" t="inlineStr"/>
-      <c r="G8" s="6" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="6" t="inlineStr"/>
-      <c r="J8" s="6" t="inlineStr"/>
-      <c r="K8" s="6" t="inlineStr"/>
-      <c r="L8" s="6" t="inlineStr"/>
-      <c r="M8" s="6" t="inlineStr"/>
-      <c r="N8" s="6" t="inlineStr"/>
-      <c r="O8" s="7" t="inlineStr"/>
-      <c r="P8" s="6" t="inlineStr"/>
-      <c r="Q8" s="6" t="inlineStr"/>
-      <c r="R8" s="6" t="inlineStr"/>
-      <c r="S8" s="6" t="inlineStr"/>
+          <t>ABF2</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>ACTCTTCCCTATCCCTTCTG</t>
+        </is>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>57.63255063313733</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>1.382550633137328</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>AGTCCTGGGATAAGAGGTG</t>
+        </is>
+      </c>
+      <c r="I8" s="6" t="n">
+        <v>57.35197420407854</v>
+      </c>
+      <c r="J8" s="6" t="n">
+        <v>1.213815269605664</v>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M8" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N8" s="6" t="n">
+        <v>2.596365902742992</v>
+      </c>
+      <c r="O8" s="7" t="inlineStr">
+        <is>
+          <t>TGGCGTAACAGGCGACACAGCACCA</t>
+        </is>
+      </c>
+      <c r="P8" s="6" t="n">
+        <v>64.69190023382828</v>
+      </c>
+      <c r="Q8" s="6" t="n">
+        <v>5.308099766171722</v>
+      </c>
+      <c r="R8" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="6" t="n">
+        <v>3.95e-06</v>
+      </c>
       <c r="T8" s="6" t="inlineStr"/>
-      <c r="U8" s="7" t="inlineStr"/>
-      <c r="V8" s="6" t="inlineStr"/>
-      <c r="W8" s="6" t="inlineStr"/>
-      <c r="X8" s="6" t="inlineStr"/>
+      <c r="U8" s="7" t="inlineStr">
+        <is>
+          <t>ACTCTTCCCTATCCCTTCTGATGACAATGGCGTAACAGGCGACACAGCACCAACGCCTAAAGCTCCAGGAATTGCAGCAGAAGCACCTTGGACAAAGCCCACATTGTTCGTTAAAGACTGATCTCCAAGTCCCACAAGACCACCACCTCTTATCCCAGGACT</t>
+        </is>
+      </c>
+      <c r="V8" s="6" t="n">
+        <v>162</v>
+      </c>
+      <c r="W8" s="6" t="n">
+        <v>50.61728395061728</v>
+      </c>
+      <c r="X8" s="6" t="n">
+        <v>-4.187627792358398</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>ILL6</t>
-        </is>
-      </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C9" s="6" t="inlineStr"/>
-      <c r="D9" s="6" t="inlineStr"/>
-      <c r="E9" s="6" t="inlineStr"/>
-      <c r="F9" s="6" t="inlineStr"/>
-      <c r="G9" s="6" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="6" t="inlineStr"/>
-      <c r="J9" s="6" t="inlineStr"/>
-      <c r="K9" s="6" t="inlineStr"/>
-      <c r="L9" s="6" t="inlineStr"/>
-      <c r="M9" s="6" t="inlineStr"/>
-      <c r="N9" s="6" t="inlineStr"/>
-      <c r="O9" s="7" t="inlineStr"/>
-      <c r="P9" s="6" t="inlineStr"/>
-      <c r="Q9" s="6" t="inlineStr"/>
-      <c r="R9" s="6" t="inlineStr"/>
-      <c r="S9" s="6" t="inlineStr"/>
+          <t>ABF2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>TCCCTATCCCTTCTGATGAC</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>57.71285363485214</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>1.462853634852138</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
+          <t>GATAAGAGGTGGTGGTCTTG</t>
+        </is>
+      </c>
+      <c r="I9" s="6" t="n">
+        <v>57.41569529783453</v>
+      </c>
+      <c r="J9" s="6" t="n">
+        <v>1.334304702165468</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="M9" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N9" s="6" t="n">
+        <v>2.797158337017606</v>
+      </c>
+      <c r="O9" s="7" t="inlineStr">
+        <is>
+          <t>TGGCGTAACAGGCGACACAGCACCA</t>
+        </is>
+      </c>
+      <c r="P9" s="6" t="n">
+        <v>64.69190023382828</v>
+      </c>
+      <c r="Q9" s="6" t="n">
+        <v>5.308099766171722</v>
+      </c>
+      <c r="R9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="6" t="n">
+        <v>3.95e-06</v>
+      </c>
       <c r="T9" s="6" t="inlineStr"/>
-      <c r="U9" s="7" t="inlineStr"/>
-      <c r="V9" s="6" t="inlineStr"/>
-      <c r="W9" s="6" t="inlineStr"/>
-      <c r="X9" s="6" t="inlineStr"/>
+      <c r="U9" s="7" t="inlineStr">
+        <is>
+          <t>TCCCTATCCCTTCTGATGACAATGGCGTAACAGGCGACACAGCACCAACGCCTAAAGCTCCAGGAATTGCAGCAGAAGCACCTTGGACAAAGCCCACATTGTTCGTTAAAGACTGATCTCCAAGTCCCACAAGACCACCACCTCTTATCC</t>
+        </is>
+      </c>
+      <c r="V9" s="6" t="n">
+        <v>149</v>
+      </c>
+      <c r="W9" s="6" t="n">
+        <v>50.66666666666667</v>
+      </c>
+      <c r="X9" s="6" t="n">
+        <v>-4.187627792358398</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>FBH2</t>
-        </is>
-      </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C10" s="6" t="inlineStr"/>
-      <c r="D10" s="6" t="inlineStr"/>
-      <c r="E10" s="6" t="inlineStr"/>
-      <c r="F10" s="6" t="inlineStr"/>
-      <c r="G10" s="6" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="6" t="inlineStr"/>
-      <c r="J10" s="6" t="inlineStr"/>
-      <c r="K10" s="6" t="inlineStr"/>
-      <c r="L10" s="6" t="inlineStr"/>
-      <c r="M10" s="6" t="inlineStr"/>
-      <c r="N10" s="6" t="inlineStr"/>
-      <c r="O10" s="7" t="inlineStr"/>
-      <c r="P10" s="6" t="inlineStr"/>
-      <c r="Q10" s="6" t="inlineStr"/>
-      <c r="R10" s="6" t="inlineStr"/>
-      <c r="S10" s="6" t="inlineStr"/>
-      <c r="T10" s="6" t="inlineStr"/>
-      <c r="U10" s="7" t="inlineStr"/>
-      <c r="V10" s="6" t="inlineStr"/>
-      <c r="W10" s="6" t="inlineStr"/>
-      <c r="X10" s="6" t="inlineStr"/>
+          <t>MAPKKK9</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>GAGTCGGAATCAGTGAAGG</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>57.24601306841157</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>1.319776405272638</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>GAAGTCGTCGGATAAGTCAC</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="n">
+        <v>57.92208372161741</v>
+      </c>
+      <c r="J10" s="6" t="n">
+        <v>1.672083721617412</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="M10" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N10" s="6" t="n">
+        <v>2.99186012689005</v>
+      </c>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <t>CGTCGCCGTGTCATGTTGCCGCA</t>
+        </is>
+      </c>
+      <c r="P10" s="6" t="n">
+        <v>64.84642607780148</v>
+      </c>
+      <c r="Q10" s="6" t="n">
+        <v>3.153573922198518</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="6" t="n">
+        <v>4.81e-05</v>
+      </c>
+      <c r="T10" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="U10" s="7" t="inlineStr">
+        <is>
+          <t>GAGTCGGAATCAGTGAAGGAAGTAGAAGAAGACACTGCGTCAGAGTTGATTTGCGTCGCCGTGTCATGTTGCCGCACCGGTGACTTATCCGACGACTTC</t>
+        </is>
+      </c>
+      <c r="V10" s="6" t="n">
+        <v>99</v>
+      </c>
+      <c r="W10" s="6" t="n">
+        <v>52.52525252525253</v>
+      </c>
+      <c r="X10" s="6" t="n">
+        <v>-5.40640926361084</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
@@ -979,67 +1321,615 @@
           <t>HCD1</t>
         </is>
       </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>No suitable primers found</t>
-        </is>
-      </c>
-      <c r="C11" s="6" t="inlineStr"/>
-      <c r="D11" s="6" t="inlineStr"/>
-      <c r="E11" s="6" t="inlineStr"/>
-      <c r="F11" s="6" t="inlineStr"/>
-      <c r="G11" s="6" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
-      <c r="I11" s="6" t="inlineStr"/>
-      <c r="J11" s="6" t="inlineStr"/>
-      <c r="K11" s="6" t="inlineStr"/>
-      <c r="L11" s="6" t="inlineStr"/>
-      <c r="M11" s="6" t="inlineStr"/>
-      <c r="N11" s="6" t="inlineStr"/>
-      <c r="O11" s="7" t="inlineStr"/>
-      <c r="P11" s="6" t="inlineStr"/>
-      <c r="Q11" s="6" t="inlineStr"/>
-      <c r="R11" s="6" t="inlineStr"/>
-      <c r="S11" s="6" t="inlineStr"/>
-      <c r="T11" s="6" t="inlineStr"/>
-      <c r="U11" s="7" t="inlineStr"/>
-      <c r="V11" s="6" t="inlineStr"/>
-      <c r="W11" s="6" t="inlineStr"/>
-      <c r="X11" s="6" t="inlineStr"/>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>GCATTGGAAGATCGAGGAG</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>57.69370414303</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>1.259493616714213</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H11" s="7" t="inlineStr">
+        <is>
+          <t>ATCCGTCCTCATCACTACC</t>
+        </is>
+      </c>
+      <c r="I11" s="6" t="n">
+        <v>57.86301338751412</v>
+      </c>
+      <c r="J11" s="6" t="n">
+        <v>1.428802861198324</v>
+      </c>
+      <c r="K11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M11" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N11" s="6" t="n">
+        <v>2.688296477912537</v>
+      </c>
+      <c r="O11" s="7" t="inlineStr">
+        <is>
+          <t>TGAGCCCACGCGAGGTCAAAGCCA</t>
+        </is>
+      </c>
+      <c r="P11" s="6" t="n">
+        <v>64.67694364829123</v>
+      </c>
+      <c r="Q11" s="6" t="n">
+        <v>4.323056351708772</v>
+      </c>
+      <c r="R11" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T11" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U11" s="7" t="inlineStr">
+        <is>
+          <t>GCATTGGAAGATCGAGGAGGGCGGCTAACACCGGTTTAAAGGATTTGACCATTTGGTGCATCCGTTTTATAGCACCGTGTCCAGCGGATTGAGCCCACGCGAGGTCAAAGCCATTGGAGAAGAACTTTCCGTGACCGGTAGTGATGAGGACGGAT</t>
+        </is>
+      </c>
+      <c r="V11" s="6" t="n">
+        <v>155</v>
+      </c>
+      <c r="W11" s="6" t="n">
+        <v>52.25806451612903</v>
+      </c>
+      <c r="X11" s="6" t="n">
+        <v>-9.328641891479492</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
+          <t>HCD1</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>GGCTAACACCGGTTTAAAGG</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>58.94711568801961</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>2.697115688019608</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H12" s="7" t="inlineStr">
+        <is>
+          <t>CTCCAATGGCTTTGACCTC</t>
+        </is>
+      </c>
+      <c r="I12" s="6" t="n">
+        <v>58.11921714417173</v>
+      </c>
+      <c r="J12" s="6" t="n">
+        <v>1.685006617855937</v>
+      </c>
+      <c r="K12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M12" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N12" s="6" t="n">
+        <v>4.382122305875544</v>
+      </c>
+      <c r="O12" s="7" t="inlineStr">
+        <is>
+          <t>CGTGTCCAGCGGATTGAGCCCACG</t>
+        </is>
+      </c>
+      <c r="P12" s="6" t="n">
+        <v>64.04111328655449</v>
+      </c>
+      <c r="Q12" s="6" t="n">
+        <v>4.958886713445509</v>
+      </c>
+      <c r="R12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T12" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U12" s="7" t="inlineStr">
+        <is>
+          <t>GGCTAACACCGGTTTAAAGGATTTGACCATTTGGTGCATCCGTTTTATAGCACCGTGTCCAGCGGATTGAGCCCACGCGAGGTCAAAGCCATTGGAGA</t>
+        </is>
+      </c>
+      <c r="V12" s="6" t="n">
+        <v>97</v>
+      </c>
+      <c r="W12" s="6" t="n">
+        <v>51.02040816326531</v>
+      </c>
+      <c r="X12" s="6" t="n">
+        <v>-6.262446403503418</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>FBH2</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>CCGGAGTATCAAGCATGTC</t>
+        </is>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>57.70037373613184</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>1.266163209816046</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H13" s="7" t="inlineStr">
+        <is>
+          <t>GTTTACCCTCTCGGCAATG</t>
+        </is>
+      </c>
+      <c r="I13" s="6" t="n">
+        <v>58.21689075554235</v>
+      </c>
+      <c r="J13" s="6" t="n">
+        <v>1.78268022922656</v>
+      </c>
+      <c r="K13" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M13" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N13" s="6" t="n">
+        <v>3.048843439042606</v>
+      </c>
+      <c r="O13" s="7" t="inlineStr">
+        <is>
+          <t>CGTGGTTGCGCAACTCATCCCCGC</t>
+        </is>
+      </c>
+      <c r="P13" s="6" t="n">
+        <v>64.97978839691598</v>
+      </c>
+      <c r="Q13" s="6" t="n">
+        <v>4.020211603084022</v>
+      </c>
+      <c r="R13" s="6" t="n">
+        <v>-0.3902359008789062</v>
+      </c>
+      <c r="S13" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T13" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="U13" s="7" t="inlineStr">
+        <is>
+          <t>CCGGAGTATCAAGCATGTCGGATATGAACATGGAGAACCTTATGGAGGACTCTGTTGCTTTTAGGGTTCGGGCTAAACGTGGTTGCGCAACTCATCCCCGCAGCATTGCCGAGAGGGTAAAC</t>
+        </is>
+      </c>
+      <c r="V13" s="6" t="n">
+        <v>122</v>
+      </c>
+      <c r="W13" s="6" t="n">
+        <v>51.63934426229508</v>
+      </c>
+      <c r="X13" s="6" t="n">
+        <v>-5.48745584487915</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>T-complex protein 11</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>CTTCTTAAGGGACCTGCTG</t>
+        </is>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>57.12484309067128</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>1.440946383012932</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H14" s="7" t="inlineStr">
+        <is>
+          <t>CAATGGTAGCGAGGAAGAC</t>
+        </is>
+      </c>
+      <c r="I14" s="6" t="n">
+        <v>57.62652924333611</v>
+      </c>
+      <c r="J14" s="6" t="n">
+        <v>1.192318717020317</v>
+      </c>
+      <c r="K14" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M14" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N14" s="6" t="n">
+        <v>2.633265100033249</v>
+      </c>
+      <c r="O14" s="7" t="inlineStr">
+        <is>
+          <t>CCAGTCGGCATGGTTCCCCAGACCA</t>
+        </is>
+      </c>
+      <c r="P14" s="6" t="n">
+        <v>64.11130686824305</v>
+      </c>
+      <c r="Q14" s="6" t="n">
+        <v>5.888693131756952</v>
+      </c>
+      <c r="R14" s="6" t="n">
+        <v>-0.3405189514160156</v>
+      </c>
+      <c r="S14" s="6" t="n">
+        <v>3.95e-06</v>
+      </c>
+      <c r="T14" s="6" t="n">
+        <v>0.08699999999999999</v>
+      </c>
+      <c r="U14" s="7" t="inlineStr">
+        <is>
+          <t>CTTCTTAAGGGACCTGCTGGTCTGGAATATCTGAAGAAGTCATTTTCCAGTCGGCATGGTTCCCCAGACCAAGCGTCTTCCTCGCTACCATTG</t>
+        </is>
+      </c>
+      <c r="V14" s="6" t="n">
+        <v>93</v>
+      </c>
+      <c r="W14" s="6" t="n">
+        <v>50.53763440860215</v>
+      </c>
+      <c r="X14" s="6" t="n">
+        <v>-6.266936302185059</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
           <t>OPT3</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
+      <c r="B15" s="7" t="inlineStr">
+        <is>
+          <t>CAGTGGTCTACTTCAGTGC</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>57.47349811284647</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>1.092291360837738</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H15" s="7" t="inlineStr">
+        <is>
+          <t>GGTCACAGGAACCATCTTC</t>
+        </is>
+      </c>
+      <c r="I15" s="6" t="n">
+        <v>57.43665772757436</v>
+      </c>
+      <c r="J15" s="6" t="n">
+        <v>1.129131746109852</v>
+      </c>
+      <c r="K15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M15" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N15" s="6" t="n">
+        <v>2.22142310694759</v>
+      </c>
+      <c r="O15" s="7" t="inlineStr">
+        <is>
+          <t>CCCATGAACGCGGTCCCTGCATCG</t>
+        </is>
+      </c>
+      <c r="P15" s="6" t="n">
+        <v>64.11877332444539</v>
+      </c>
+      <c r="Q15" s="6" t="n">
+        <v>4.881226675554615</v>
+      </c>
+      <c r="R15" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T15" s="6" t="inlineStr"/>
+      <c r="U15" s="7" t="inlineStr">
+        <is>
+          <t>CAGTGGTCTACTTCAGTGCCCCACCATTTGAGGTCGTGTCCAGCATTCTGCAGGGCGAAGAACAAGAGCACCCCCATGAACGCGGTCCCTGCATCGAGCGCTGCAGAGAGTACGTAATTGTACTTCTGCCACCATCTCTTGTGGTAATTGAACACAAAGTAGTTGAAGATGGTTCCTGTGACC</t>
+        </is>
+      </c>
+      <c r="V15" s="6" t="n">
+        <v>183</v>
+      </c>
+      <c r="W15" s="6" t="n">
+        <v>51.91256830601093</v>
+      </c>
+      <c r="X15" s="6" t="n">
+        <v>-9.127151489257812</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>OPT3</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="inlineStr">
+        <is>
+          <t>CATTTGAGGTCGTGTCCAG</t>
+        </is>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>58.15230648873609</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>1.718095962420296</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H16" s="7" t="inlineStr">
+        <is>
+          <t>GAGATGGTGGCAGAAGTAC</t>
+        </is>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>57.22615453006745</v>
+      </c>
+      <c r="J16" s="6" t="n">
+        <v>1.339634943616762</v>
+      </c>
+      <c r="K16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M16" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>3.057730906037058</v>
+      </c>
+      <c r="O16" s="7" t="inlineStr">
+        <is>
+          <t>CCCATGAACGCGGTCCCTGCATCG</t>
+        </is>
+      </c>
+      <c r="P16" s="6" t="n">
+        <v>64.11877332444539</v>
+      </c>
+      <c r="Q16" s="6" t="n">
+        <v>4.881226675554615</v>
+      </c>
+      <c r="R16" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T16" s="6" t="inlineStr"/>
+      <c r="U16" s="7" t="inlineStr">
+        <is>
+          <t>CATTTGAGGTCGTGTCCAGCATTCTGCAGGGCGAAGAACAAGAGCACCCCCATGAACGCGGTCCCTGCATCGAGCGCTGCAGAGAGTACGTAATTGTACTTCTGCCACCATCTCT</t>
+        </is>
+      </c>
+      <c r="V16" s="6" t="n">
+        <v>114</v>
+      </c>
+      <c r="W16" s="6" t="n">
+        <v>54.78260869565217</v>
+      </c>
+      <c r="X16" s="6" t="n">
+        <v>-7.249449729919434</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>OPT3</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="inlineStr">
+        <is>
+          <t>CACCATTTGAGGTCGTGTC</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>58.4545610961726</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>2.020350569856806</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H17" s="7" t="inlineStr">
+        <is>
+          <t>CAAGAGATGGTGGCAGAAG</t>
+        </is>
+      </c>
+      <c r="I17" s="6" t="n">
+        <v>57.82604913973512</v>
+      </c>
+      <c r="J17" s="6" t="n">
+        <v>1.391838613419328</v>
+      </c>
+      <c r="K17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="M17" s="6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <v>3.412189183276134</v>
+      </c>
+      <c r="O17" s="7" t="inlineStr">
+        <is>
+          <t>CCCATGAACGCGGTCCCTGCATCG</t>
+        </is>
+      </c>
+      <c r="P17" s="6" t="n">
+        <v>64.11877332444539</v>
+      </c>
+      <c r="Q17" s="6" t="n">
+        <v>4.881226675554615</v>
+      </c>
+      <c r="R17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="6" t="n">
+        <v>1.38e-05</v>
+      </c>
+      <c r="T17" s="6" t="inlineStr"/>
+      <c r="U17" s="7" t="inlineStr">
+        <is>
+          <t>CACCATTTGAGGTCGTGTCCAGCATTCTGCAGGGCGAAGAACAAGAGCACCCCCATGAACGCGGTCCCTGCATCGAGCGCTGCAGAGAGTACGTAATTGTACTTCTGCCACCATCTCTTGT</t>
+        </is>
+      </c>
+      <c r="V17" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="W17" s="6" t="n">
+        <v>54.54545454545454</v>
+      </c>
+      <c r="X17" s="6" t="n">
+        <v>-7.249449729919434</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>GA20OX5</t>
+        </is>
+      </c>
+      <c r="B18" s="8" t="inlineStr">
         <is>
           <t>No suitable primers found</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr"/>
-      <c r="D12" s="6" t="inlineStr"/>
-      <c r="E12" s="6" t="inlineStr"/>
-      <c r="F12" s="6" t="inlineStr"/>
-      <c r="G12" s="6" t="inlineStr"/>
-      <c r="H12" s="7" t="inlineStr"/>
-      <c r="I12" s="6" t="inlineStr"/>
-      <c r="J12" s="6" t="inlineStr"/>
-      <c r="K12" s="6" t="inlineStr"/>
-      <c r="L12" s="6" t="inlineStr"/>
-      <c r="M12" s="6" t="inlineStr"/>
-      <c r="N12" s="6" t="inlineStr"/>
-      <c r="O12" s="7" t="inlineStr"/>
-      <c r="P12" s="6" t="inlineStr"/>
-      <c r="Q12" s="6" t="inlineStr"/>
-      <c r="R12" s="6" t="inlineStr"/>
-      <c r="S12" s="6" t="inlineStr"/>
-      <c r="T12" s="6" t="inlineStr"/>
-      <c r="U12" s="7" t="inlineStr"/>
-      <c r="V12" s="6" t="inlineStr"/>
-      <c r="W12" s="6" t="inlineStr"/>
-      <c r="X12" s="6" t="inlineStr"/>
+      <c r="C18" s="6" t="inlineStr"/>
+      <c r="D18" s="6" t="inlineStr"/>
+      <c r="E18" s="6" t="inlineStr"/>
+      <c r="F18" s="6" t="inlineStr"/>
+      <c r="G18" s="6" t="inlineStr"/>
+      <c r="H18" s="7" t="inlineStr"/>
+      <c r="I18" s="6" t="inlineStr"/>
+      <c r="J18" s="6" t="inlineStr"/>
+      <c r="K18" s="6" t="inlineStr"/>
+      <c r="L18" s="6" t="inlineStr"/>
+      <c r="M18" s="6" t="inlineStr"/>
+      <c r="N18" s="6" t="inlineStr"/>
+      <c r="O18" s="7" t="inlineStr"/>
+      <c r="P18" s="6" t="inlineStr"/>
+      <c r="Q18" s="6" t="inlineStr"/>
+      <c r="R18" s="6" t="inlineStr"/>
+      <c r="S18" s="6" t="inlineStr"/>
+      <c r="T18" s="6" t="inlineStr"/>
+      <c r="U18" s="7" t="inlineStr"/>
+      <c r="V18" s="6" t="inlineStr"/>
+      <c r="W18" s="6" t="inlineStr"/>
+      <c r="X18" s="6" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>